<commit_message>
2019-04-24 MRI Project Developing
</commit_message>
<xml_diff>
--- a/HH_Projects/01_Market_Risk_Indicator/Data_Files/Source_Files/msci_reclassifications.xlsx
+++ b/HH_Projects/01_Market_Risk_Indicator/Data_Files/Source_Files/msci_reclassifications.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Job\Projects\01 - Market Risk\MRI_Data\MSCI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Job\GitHub Repository\HH_Codebase\HH_Projects\01_Market_Risk_Indicator\Data_Files\Source_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B978431-996E-4791-BE01-453B76B0774F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFD3493-8244-4036-9C50-57F930AB405C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C2C50C80-435C-4B5B-9178-B6ED70AD141F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C2C50C80-435C-4B5B-9178-B6ED70AD141F}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>August 2016</t>
   </si>
@@ -97,9 +97,6 @@
     <t>May 2014</t>
   </si>
   <si>
-    <t>MSCI UAE Index</t>
-  </si>
-  <si>
     <t>MSCI Greece Index</t>
   </si>
   <si>
@@ -200,6 +197,12 @@
   </si>
   <si>
     <t>June 2001</t>
+  </si>
+  <si>
+    <t>MSCI UNITED ARAB EMIRATES Index</t>
+  </si>
+  <si>
+    <t>3) Rename "UAE" to "United Arab Emirates"</t>
   </si>
 </sst>
 </file>
@@ -299,11 +302,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -619,33 +622,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55213165-522E-4380-8209-AEAC8F6A6804}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="B2" t="s">
         <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -661,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85022744-85FC-45FF-96A6-031E6EC869EE}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,11 +679,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -761,7 +769,7 @@
     </row>
     <row r="10" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>21</v>
@@ -772,189 +780,189 @@
     </row>
     <row r="11" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2019-04-26 MRI project developing
</commit_message>
<xml_diff>
--- a/HH_Projects/01_Market_Risk_Indicator/Data_Files/Source_Files/msci_reclassifications.xlsx
+++ b/HH_Projects/01_Market_Risk_Indicator/Data_Files/Source_Files/msci_reclassifications.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Job\GitHub Repository\HH_Codebase\HH_Projects\01_Market_Risk_Indicator\Data_Files\Source_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFD3493-8244-4036-9C50-57F930AB405C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4102D007-79D0-4F18-95A6-8C2F33F0BF8D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C2C50C80-435C-4B5B-9178-B6ED70AD141F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Instructions" sheetId="2" r:id="rId1"/>
-    <sheet name="Reclassifications" sheetId="1" r:id="rId2"/>
+    <sheet name="Reclassifications" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
   <si>
     <t>August 2016</t>
   </si>
@@ -175,21 +174,6 @@
     <t>November 1997</t>
   </si>
   <si>
-    <t>URL:</t>
-  </si>
-  <si>
-    <t>Actions:</t>
-  </si>
-  <si>
-    <t>1) Name source tab 'Reclassifications'</t>
-  </si>
-  <si>
-    <t>https://www.msci.com/market-classification</t>
-  </si>
-  <si>
-    <t>2) Add rows from annotations</t>
-  </si>
-  <si>
     <t>December 2008</t>
   </si>
   <si>
@@ -200,16 +184,13 @@
   </si>
   <si>
     <t>MSCI UNITED ARAB EMIRATES Index</t>
-  </si>
-  <si>
-    <t>3) Rename "UAE" to "United Arab Emirates"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,15 +229,6 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -285,7 +257,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -302,8 +274,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -621,55 +591,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55213165-522E-4380-8209-AEAC8F6A6804}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{B1043A55-91AA-42EF-8D5F-68817BA53654}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85022744-85FC-45FF-96A6-031E6EC869EE}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -679,11 +604,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -769,7 +694,7 @@
     </row>
     <row r="10" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>21</v>
@@ -948,10 +873,10 @@
         <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
@@ -959,10 +884,10 @@
         <v>41</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>